<commit_message>
cleaned it up a little
</commit_message>
<xml_diff>
--- a/4site/4site_nearest.xlsx
+++ b/4site/4site_nearest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="32500" windowHeight="20800" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="100" yWindow="240" windowWidth="36720" windowHeight="20900" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,9 @@
     <sheet name="5" sheetId="6" r:id="rId6"/>
     <sheet name="6" sheetId="7" r:id="rId7"/>
     <sheet name="7" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'2'!$A$2:$Q$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'2'!$B$2:$R$29</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -4291,8 +4290,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4498,7 +4501,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4529,6 +4532,8 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4559,6 +4564,8 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9766,7 +9773,7 @@
   <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9876,907 +9883,956 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="17" width="7.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="18" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="9" customHeight="1"/>
-    <row r="2" spans="1:17" ht="16" thickBot="1">
-      <c r="A2" t="s">
+    <row r="1" spans="1:18" ht="9" customHeight="1"/>
+    <row r="2" spans="1:18" ht="16" thickBot="1">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="33" customHeight="1">
-      <c r="A3" s="9" t="str">
-        <f>B2</f>
+    <row r="3" spans="1:18" ht="33" customHeight="1">
+      <c r="B3" s="9" t="str">
+        <f>C2</f>
         <v></v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="I3" s="11" t="str">
-        <f>J2</f>
+      <c r="C3" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="J3" s="11" t="str">
+        <f>K2</f>
         <v></v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:17" ht="33" customHeight="1">
-      <c r="A4" s="9" t="str">
-        <f>C2</f>
+      <c r="K3" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:18" ht="33" customHeight="1">
+      <c r="B4" s="9" t="str">
+        <f>D2</f>
         <v></v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>277</v>
+      <c r="C4" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>278</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="I4" s="11" t="str">
-        <f>K2</f>
+      <c r="F4" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="J4" s="11" t="str">
+        <f>L2</f>
         <v></v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>277</v>
+      <c r="K4" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>278</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="33" customHeight="1">
-      <c r="A5" s="9" t="str">
-        <f>D2</f>
+      <c r="N4" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="33" customHeight="1">
+      <c r="B5" s="9" t="str">
+        <f>E2</f>
         <v></v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="I5" s="11" t="str">
-        <f>L2</f>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="J5" s="11" t="str">
+        <f>M2</f>
         <v></v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="O5" s="19"/>
-      <c r="Q5" t="s">
+      <c r="K5" s="16"/>
+      <c r="L5" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="R5" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="33" customHeight="1">
-      <c r="A6" s="9" t="str">
-        <f>E2</f>
+    <row r="6" spans="1:18" ht="33" customHeight="1">
+      <c r="B6" s="9" t="str">
+        <f>F2</f>
         <v></v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="I6" s="11" t="str">
-        <f>M2</f>
+      <c r="C6" s="20"/>
+      <c r="D6" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="J6" s="11" t="str">
+        <f>N2</f>
         <v></v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="O6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" ht="33" customHeight="1">
-      <c r="A7" s="9" t="str">
-        <f>F2</f>
+      <c r="K6" s="20"/>
+      <c r="L6" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="P6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" ht="33" customHeight="1">
+      <c r="B7" s="9" t="str">
+        <f>G2</f>
         <v></v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>277</v>
-      </c>
+      <c r="C7" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="17"/>
       <c r="E7" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="I7" s="11" t="str">
-        <f>N2</f>
+      <c r="F7" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="J7" s="11" t="str">
+        <f>O2</f>
         <v></v>
       </c>
-      <c r="J7" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17" t="s">
-        <v>277</v>
-      </c>
+      <c r="K7" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="L7" s="17"/>
       <c r="M7" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="N7" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="33" customHeight="1" thickBot="1">
-      <c r="A8" s="9" t="str">
-        <f>G2</f>
+      <c r="N7" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="33" customHeight="1" thickBot="1">
+      <c r="B8" s="9" t="str">
+        <f>H2</f>
         <v></v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>278</v>
-      </c>
-      <c r="I8" s="11" t="str">
-        <f>O2</f>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="J8" s="11" t="str">
+        <f>P2</f>
         <v></v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="9" customHeight="1">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="7" customHeight="1">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="B11" t="s">
+      <c r="K8" s="21"/>
+      <c r="L8" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="M8" s="23"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="9" customHeight="1">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="7" customHeight="1">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="C11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="9" customHeight="1"/>
-    <row r="13" spans="1:17" ht="16" thickBot="1">
-      <c r="A13" t="s">
+    <row r="12" spans="1:18" ht="9" customHeight="1"/>
+    <row r="13" spans="1:18" ht="16" thickBot="1">
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="31" customHeight="1">
-      <c r="A14" s="4" t="str">
-        <f>B13</f>
+    <row r="14" spans="1:18" ht="31" customHeight="1">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <f>C13</f>
         <v></v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="E14" s="13"/>
+      <c r="C14" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>277</v>
+      </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="L14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14" t="s">
+        <v>277</v>
+      </c>
       <c r="M14" s="13"/>
-      <c r="N14" s="13" t="s">
-        <v>277</v>
-      </c>
+      <c r="N14" s="13"/>
       <c r="O14" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="15"/>
-    </row>
-    <row r="15" spans="1:17" ht="31" customHeight="1">
-      <c r="A15" s="4" t="str">
-        <f>C13</f>
+      <c r="P14" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="15"/>
+    </row>
+    <row r="15" spans="1:18" ht="31" customHeight="1">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f>D13</f>
         <v></v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="F15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="K15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="25" t="s">
-        <v>277</v>
-      </c>
+      <c r="N15" s="17"/>
       <c r="O15" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="19"/>
-    </row>
-    <row r="16" spans="1:17" ht="31" customHeight="1">
-      <c r="A16" s="4" t="str">
-        <f>D13</f>
+      <c r="P15" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="19"/>
+    </row>
+    <row r="16" spans="1:18" ht="31" customHeight="1">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <f>E13</f>
         <v></v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="I16" s="17"/>
+      <c r="C16" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="N16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="19"/>
-    </row>
-    <row r="17" spans="1:17" ht="31" customHeight="1">
-      <c r="A17" s="4" t="str">
-        <f>E13</f>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="19"/>
+    </row>
+    <row r="17" spans="1:18" ht="31" customHeight="1">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4" t="str">
+        <f>F13</f>
         <v></v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="J17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="K17" s="17"/>
-      <c r="L17" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="19"/>
-    </row>
-    <row r="18" spans="1:17" ht="31" customHeight="1">
-      <c r="A18" s="4" t="str">
-        <f>F13</f>
+      <c r="L17" s="17"/>
+      <c r="M17" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="19"/>
+    </row>
+    <row r="18" spans="1:18" ht="31" customHeight="1">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <f>G13</f>
         <v></v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="G18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="K18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="O18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="P18" s="17"/>
-      <c r="Q18" s="19" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="31" customHeight="1">
-      <c r="A19" s="4" t="str">
-        <f>G13</f>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="19" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="31" customHeight="1">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f>H13</f>
         <v></v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="17"/>
-      <c r="E19" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="H19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="L19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="M19" s="17"/>
-      <c r="N19" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="O19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="P19" s="17"/>
-      <c r="Q19" s="18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="31" customHeight="1">
-      <c r="A20" s="4" t="str">
-        <f>H13</f>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="31" customHeight="1">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f>I13</f>
         <v></v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="E20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="K20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="L20" s="17"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17" t="s">
-        <v>277</v>
-      </c>
+      <c r="M20" s="17"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="17"/>
       <c r="P20" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="Q20" s="19"/>
-    </row>
-    <row r="21" spans="1:17" ht="31" customHeight="1">
-      <c r="A21" s="4" t="str">
-        <f>I13</f>
+      <c r="Q20" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="R20" s="19"/>
+    </row>
+    <row r="21" spans="1:18" ht="31" customHeight="1">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f>J13</f>
         <v></v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="F21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="L21" s="25"/>
-      <c r="M21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="25" t="s">
-        <v>277</v>
-      </c>
+      <c r="O21" s="17"/>
       <c r="P21" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="Q21" s="19"/>
-    </row>
-    <row r="22" spans="1:17" ht="31" customHeight="1">
-      <c r="A22" s="4" t="str">
-        <f>J13</f>
+      <c r="Q21" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="R21" s="19"/>
+    </row>
+    <row r="22" spans="1:18" ht="31" customHeight="1">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <f>K13</f>
         <v></v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="E22" s="17"/>
-      <c r="F22" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="M22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17" t="s">
+        <v>277</v>
+      </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="19"/>
-    </row>
-    <row r="23" spans="1:17" ht="31" customHeight="1">
-      <c r="A23" s="4" t="str">
-        <f>K13</f>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="19"/>
+    </row>
+    <row r="23" spans="1:18" ht="31" customHeight="1">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="str">
+        <f>L13</f>
         <v></v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="20" t="s">
+        <v>277</v>
+      </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="N23" s="17"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="18"/>
-    </row>
-    <row r="24" spans="1:17" ht="31" customHeight="1">
-      <c r="A24" s="4" t="str">
-        <f>L13</f>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="O23" s="17"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="18"/>
+    </row>
+    <row r="24" spans="1:18" ht="31" customHeight="1">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <f>M13</f>
         <v></v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="F24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="M24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
-      <c r="P24" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q24" s="19" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="31" customHeight="1">
-      <c r="A25" s="4" t="str">
-        <f>M13</f>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="31" customHeight="1">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4" t="str">
+        <f>N13</f>
         <v></v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="E25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="25"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="N25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="O25" s="17"/>
-      <c r="P25" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q25" s="18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="31" customHeight="1">
-      <c r="A26" s="4" t="str">
-        <f>N13</f>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="R25" s="18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="31" customHeight="1">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f>O13</f>
         <v>✖</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="H26" s="17"/>
+      <c r="C26" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="O26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="P26" s="17"/>
-      <c r="Q26" s="19"/>
-    </row>
-    <row r="27" spans="1:17" ht="31" customHeight="1">
-      <c r="A27" s="4" t="str">
-        <f>O13</f>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="19"/>
+    </row>
+    <row r="27" spans="1:18" ht="31" customHeight="1">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f>P13</f>
         <v>✖</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D27" s="17"/>
+      <c r="C27" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="25"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
-      <c r="O27" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="19"/>
-    </row>
-    <row r="28" spans="1:17" ht="31" customHeight="1">
-      <c r="A28" s="4" t="str">
-        <f>P13</f>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="19"/>
+    </row>
+    <row r="28" spans="1:18" ht="31" customHeight="1">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <f>Q13</f>
         <v>✖</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="J28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="K28" s="17"/>
-      <c r="L28" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="N28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="N28" s="25" t="s">
+        <v>277</v>
+      </c>
       <c r="O28" s="17"/>
-      <c r="P28" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q28" s="19"/>
-    </row>
-    <row r="29" spans="1:17" ht="31" customHeight="1" thickBot="1">
-      <c r="A29" s="4" t="str">
-        <f>Q13</f>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="R28" s="19"/>
+    </row>
+    <row r="29" spans="1:18" ht="31" customHeight="1" thickBot="1">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4" t="str">
+        <f>R13</f>
         <v>✖</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="23"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="H29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>277</v>
+      </c>
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="M29" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="N29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>277</v>
+      </c>
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
-      <c r="Q29" s="24" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="4"/>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="4"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="4"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="4"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
@@ -10794,8 +10850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA97"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13360,8 +13416,8 @@
   </sheetPr>
   <dimension ref="A1:AK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19921,7 +19977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -20022,21 +20078,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>